<commit_message>
ECP-985: takes currency out of erv model; adds new erv actions on unit; cosmetic changes
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/asset/fixtures/erv/ERVImport.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/asset/fixtures/erv/ERVImport.xlsx
@@ -19,15 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>OXF-001</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>GBP</t>
   </si>
   <si>
     <t>Type</t>
@@ -46,9 +40,6 @@
   </si>
   <si>
     <t>Value</t>
-  </si>
-  <si>
-    <t>Currency Reference</t>
   </si>
 </sst>
 </file>
@@ -705,7 +696,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -719,20 +710,18 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
@@ -742,13 +731,10 @@
         <v>43466</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2">
         <v>14814.68</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -759,13 +745,10 @@
         <v>43556</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2">
         <v>2345.6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -776,13 +759,10 @@
         <v>43191</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2">
         <v>13000.55</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>